<commit_message>
released revised Formative09, xlookup intro
</commit_message>
<xml_diff>
--- a/Formative09/xLookup.xlsx
+++ b/Formative09/xLookup.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mnscu-my.sharepoint.com/personal/wp8798rh_minnstate_edu/Documents/GitHub/eprof1/MIS362-03/Formative09/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wp8798rh\OneDrive - MNSCU\GitHub\eprof1\MIS362-03\Formative09\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{C447C971-B65C-4488-A6FD-D1A5AD15F95F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5164BEE1-6F81-46AE-A50B-1731AB966AD0}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{B4479C1E-D018-433D-8F9F-34D1891D027D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EE499058-9269-4166-B55F-FC259E98F2FE}"/>
   <bookViews>
-    <workbookView xWindow="-370" yWindow="-21710" windowWidth="38620" windowHeight="21360" xr2:uid="{DD1172EC-2C53-41E4-BE0E-3D966464F75B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{DD1172EC-2C53-41E4-BE0E-3D966464F75B}"/>
   </bookViews>
   <sheets>
     <sheet name="Latest Order" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2354" uniqueCount="2327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2355" uniqueCount="2328">
   <si>
     <t>Transaction Date</t>
   </si>
@@ -7019,7 +7019,10 @@
     <t>AX3429694</t>
   </si>
   <si>
-    <t>&lt;-- when was gift card last used?</t>
+    <t>&lt;-- find when  gift card was last used</t>
+  </si>
+  <si>
+    <t>Use the xlookup() function</t>
   </si>
 </sst>
 </file>
@@ -7554,16 +7557,16 @@
   <dimension ref="B1:L2345"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="141" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.19921875" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.09765625" customWidth="1"/>
-    <col min="4" max="4" width="3.19921875" customWidth="1"/>
-    <col min="5" max="5" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.09765625" customWidth="1"/>
+    <col min="4" max="4" width="2.5" customWidth="1"/>
+    <col min="5" max="5" width="29.8984375" customWidth="1"/>
     <col min="6" max="6" width="1.69921875" customWidth="1"/>
     <col min="7" max="7" width="18.8984375" customWidth="1"/>
     <col min="8" max="8" width="13.19921875" customWidth="1"/>
@@ -7611,10 +7614,7 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4">
-        <f>_xlfn.XLOOKUP(B4,'Latest Order'!$H$3:$H$2344,'Latest Order'!$G$3:$G$2344,"not used",,-1)</f>
-        <v>43241</v>
-      </c>
+      <c r="C4" s="4"/>
       <c r="E4" t="s">
         <v>2326</v>
       </c>
@@ -7632,9 +7632,9 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4" t="str">
-        <f>_xlfn.XLOOKUP(B5,'Latest Order'!$H$3:$H$2344,'Latest Order'!$G$3:$G$2344,"not used",,-1)</f>
-        <v>not used</v>
+      <c r="C5" s="4"/>
+      <c r="E5" t="s">
+        <v>2327</v>
       </c>
       <c r="G5" s="12">
         <v>42201</v>
@@ -7650,10 +7650,7 @@
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4">
-        <f>_xlfn.XLOOKUP(B6,'Latest Order'!$H$3:$H$2344,'Latest Order'!$G$3:$G$2344,"not used",,-1)</f>
-        <v>42971</v>
-      </c>
+      <c r="C6" s="4"/>
       <c r="G6" s="12">
         <v>42201</v>
       </c>
@@ -7668,10 +7665,7 @@
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4">
-        <f>_xlfn.XLOOKUP(B7,'Latest Order'!$H$3:$H$2344,'Latest Order'!$G$3:$G$2344,"not used",,-1)</f>
-        <v>42294</v>
-      </c>
+      <c r="C7" s="4"/>
       <c r="G7" s="12">
         <v>42201</v>
       </c>
@@ -7686,10 +7680,7 @@
       <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4">
-        <f>_xlfn.XLOOKUP(B8,'Latest Order'!$H$3:$H$2344,'Latest Order'!$G$3:$G$2344,"not used",,-1)</f>
-        <v>42642</v>
-      </c>
+      <c r="C8" s="4"/>
       <c r="G8" s="12">
         <v>42203</v>
       </c>
@@ -7705,10 +7696,7 @@
       <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="4">
-        <f>_xlfn.XLOOKUP(B9,'Latest Order'!$H$3:$H$2344,'Latest Order'!$G$3:$G$2344,"not used",,-1)</f>
-        <v>43869</v>
-      </c>
+      <c r="C9" s="4"/>
       <c r="G9" s="12">
         <v>42203</v>
       </c>
@@ -33416,6 +33404,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E0C6E51200D864478E07966DED5DCEDD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cf7312fb2f3a2b8ec40c186e3d2471cc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e5c8654-c470-41ab-8181-ffc61620d570" xmlns:ns4="f02ba748-faeb-47bc-8c82-1c0f8806a7db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b93dd8c237d26b2edead1677503bd446" ns3:_="" ns4:_="">
     <xsd:import namespace="0e5c8654-c470-41ab-8181-ffc61620d570"/>
@@ -33638,22 +33641,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F02FDCC-3482-484E-A31F-E9011A13D78E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFC1F3CA-D879-42F1-A3F4-B789A0CBB757}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1EAB567-C45F-43B2-A854-26491718E8A2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33670,21 +33675,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F02FDCC-3482-484E-A31F-E9011A13D78E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFC1F3CA-D879-42F1-A3F4-B789A0CBB757}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>